<commit_message>
amended formatting in tables
</commit_message>
<xml_diff>
--- a/write/tables/tb_occupancy_effects_reco.xlsx
+++ b/write/tables/tb_occupancy_effects_reco.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23400" windowHeight="17920"/>
+    <workbookView xWindow="0" yWindow="9180" windowWidth="28800" windowHeight="8740"/>
   </bookViews>
   <sheets>
     <sheet name="formatted" sheetId="3" r:id="rId1"/>
     <sheet name="varsBy_room_cmp2" sheetId="1" r:id="rId2"/>
     <sheet name="varsBy_room_cmp2_detail" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="296">
   <si>
     <t>varname</t>
   </si>
@@ -875,15 +875,6 @@
   </si>
   <si>
     <t>Patients assessed (% of sample)</t>
-  </si>
-  <si>
-    <t>(8%)</t>
-  </si>
-  <si>
-    <t>(24%)</t>
-  </si>
-  <si>
-    <t>(69%)</t>
   </si>
   <si>
     <t>Accepted to critical care</t>
@@ -932,7 +923,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -943,6 +934,27 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -985,7 +997,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
       <alignment wrapText="1"/>
@@ -1002,55 +1014,95 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="20">
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="XLConnect.Boolean" xfId="4"/>
     <cellStyle name="XLConnect.DateTime" xfId="5"/>
@@ -1331,19 +1383,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:K18"/>
+  <dimension ref="B3:K19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="34.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="str">
         <f>varsBy_room_cmp2!A2</f>
@@ -1369,441 +1423,456 @@
         <v>281</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B4" s="8" t="s">
         <v>282</v>
       </c>
-      <c r="C4" s="7" t="str">
+      <c r="C4" s="8" t="str">
         <f>varsBy_room_cmp2!A3</f>
         <v>icu_accept</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <f>varsBy_room_cmp2!B3</f>
         <v>1</v>
       </c>
-      <c r="E4" s="8" t="str">
+      <c r="E4" s="9" t="str">
+        <f>varsBy_room_cmp2!C2</f>
+        <v>376</v>
+      </c>
+      <c r="F4" s="19" t="str">
+        <f>CONCATENATE("(",ROUND(VALUE(E4)/SUM(VALUE($E4),VALUE($G4),VALUE($I4))*100,0),"%)")</f>
+        <v>(8%)</v>
+      </c>
+      <c r="G4" s="9" t="str">
+        <f>varsBy_room_cmp2!E2</f>
+        <v>1175</v>
+      </c>
+      <c r="H4" s="19" t="str">
+        <f>CONCATENATE("(",ROUND(VALUE(G4)/SUM(VALUE($E4),VALUE($G4),VALUE($I4))*100,0),"%)")</f>
+        <v>(24%)</v>
+      </c>
+      <c r="I4" s="9" t="str">
+        <f>varsBy_room_cmp2!G2</f>
+        <v>3421</v>
+      </c>
+      <c r="J4" s="19" t="str">
+        <f>CONCATENATE("(",ROUND(VALUE(I4)/SUM(VALUE($E4),VALUE($G4),VALUE($I4))*100,0),"%)")</f>
+        <v>(69%)</v>
+      </c>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B6" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C6" s="10" t="str">
+        <f>varsBy_room_cmp2!A4</f>
+        <v>icu_accept</v>
+      </c>
+      <c r="D6" s="10">
+        <f>varsBy_room_cmp2!B4</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="22" t="str">
         <f>varsBy_room_cmp2!C3</f>
         <v>194</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="G4" s="8" t="str">
+      <c r="F6" s="23" t="str">
+        <f>varsBy_room_cmp2!D3</f>
+        <v>(51.6%)</v>
+      </c>
+      <c r="G6" s="22" t="str">
         <f>varsBy_room_cmp2!E3</f>
         <v>727</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="I4" s="8" t="str">
+      <c r="H6" s="23" t="str">
+        <f>varsBy_room_cmp2!F3</f>
+        <v>(61.9%)</v>
+      </c>
+      <c r="I6" s="22" t="str">
         <f>varsBy_room_cmp2!G3</f>
         <v>2454</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="C5" s="11" t="str">
-        <f>varsBy_room_cmp2!A4</f>
-        <v>icu_accept</v>
-      </c>
-      <c r="D5" s="11">
-        <f>varsBy_room_cmp2!B4</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="12" t="str">
-        <f>varsBy_room_cmp2!C4</f>
-        <v>182</v>
-      </c>
-      <c r="F5" s="11" t="str">
-        <f>varsBy_room_cmp2!D4</f>
-        <v>(48.4%)</v>
-      </c>
-      <c r="G5" s="13" t="str">
-        <f>varsBy_room_cmp2!E4</f>
-        <v>448</v>
-      </c>
-      <c r="H5" s="11" t="str">
-        <f>varsBy_room_cmp2!F4</f>
-        <v>(38.1%)</v>
-      </c>
-      <c r="I5" s="13" t="str">
-        <f>varsBy_room_cmp2!G4</f>
-        <v>967</v>
-      </c>
-      <c r="J5" s="11" t="str">
-        <f>varsBy_room_cmp2!H4</f>
-        <v>(28.3%)</v>
-      </c>
-      <c r="K5" s="13">
-        <f>varsBy_room_cmp2!L4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C6" t="str">
+      <c r="J6" s="23" t="str">
+        <f>varsBy_room_cmp2!H3</f>
+        <v>(71.7%)</v>
+      </c>
+      <c r="K6" s="12" t="str">
+        <f>varsBy_room_cmp2!L3</f>
+        <v>&lt;0.0001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B7" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="7" t="str">
         <f>varsBy_room_cmp2!A6</f>
         <v>early4.ok</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="7">
         <f>varsBy_room_cmp2!B6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="14" t="str">
-        <f>varsBy_room_cmp2!C6</f>
-        <v>294</v>
-      </c>
-      <c r="F6" t="str">
-        <f>varsBy_room_cmp2!D6</f>
-        <v>(78.2%)</v>
-      </c>
-      <c r="G6" s="15" t="str">
-        <f>varsBy_room_cmp2!E6</f>
-        <v>747</v>
-      </c>
-      <c r="H6" t="str">
-        <f>varsBy_room_cmp2!F6</f>
-        <v>(63.6%)</v>
-      </c>
-      <c r="I6" s="15" t="str">
-        <f>varsBy_room_cmp2!G6</f>
-        <v>1676</v>
-      </c>
-      <c r="J6" t="str">
-        <f>varsBy_room_cmp2!H6</f>
-        <v>(49.0%)</v>
-      </c>
-      <c r="K6" s="15">
-        <f>varsBy_room_cmp2!L6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="C7" s="11" t="str">
+      <c r="E7" s="9" t="str">
+        <f>varsBy_room_cmp2!C5</f>
+        <v>82</v>
+      </c>
+      <c r="F7" s="20" t="str">
+        <f>varsBy_room_cmp2!D5</f>
+        <v>(21.8%)</v>
+      </c>
+      <c r="G7" s="9" t="str">
+        <f>varsBy_room_cmp2!E5</f>
+        <v>428</v>
+      </c>
+      <c r="H7" s="20" t="str">
+        <f>varsBy_room_cmp2!F5</f>
+        <v>(36.4%)</v>
+      </c>
+      <c r="I7" s="9" t="str">
+        <f>varsBy_room_cmp2!G5</f>
+        <v>1745</v>
+      </c>
+      <c r="J7" s="20" t="str">
+        <f>varsBy_room_cmp2!H5</f>
+        <v>(51.0%)</v>
+      </c>
+      <c r="K7" s="21" t="str">
+        <f>varsBy_room_cmp2!L5</f>
+        <v>&lt;0.0001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B8" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="10" t="str">
         <f>varsBy_room_cmp2!A8</f>
         <v>icucmp</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D8" s="10">
         <f>varsBy_room_cmp2!B8</f>
         <v>0</v>
       </c>
-      <c r="E7" s="12" t="str">
-        <f>varsBy_room_cmp2!C8</f>
-        <v>175</v>
-      </c>
-      <c r="F7" s="11" t="str">
-        <f>varsBy_room_cmp2!D8</f>
-        <v>(46.5%)</v>
-      </c>
-      <c r="G7" s="13" t="str">
-        <f>varsBy_room_cmp2!E8</f>
-        <v>372</v>
-      </c>
-      <c r="H7" s="11" t="str">
-        <f>varsBy_room_cmp2!F8</f>
-        <v>(31.7%)</v>
-      </c>
-      <c r="I7" s="13" t="str">
-        <f>varsBy_room_cmp2!G8</f>
-        <v>734</v>
-      </c>
-      <c r="J7" s="11" t="str">
-        <f>varsBy_room_cmp2!H8</f>
-        <v>(21.5%)</v>
-      </c>
-      <c r="K7" s="13">
-        <f>varsBy_room_cmp2!L8</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>289</v>
-      </c>
-      <c r="C8" t="str">
+      <c r="E8" s="22" t="str">
+        <f>varsBy_room_cmp2!C7</f>
+        <v>201</v>
+      </c>
+      <c r="F8" s="23" t="str">
+        <f>varsBy_room_cmp2!D7</f>
+        <v>(53.5%)</v>
+      </c>
+      <c r="G8" s="22" t="str">
+        <f>varsBy_room_cmp2!E7</f>
+        <v>803</v>
+      </c>
+      <c r="H8" s="23" t="str">
+        <f>varsBy_room_cmp2!F7</f>
+        <v>(68.3%)</v>
+      </c>
+      <c r="I8" s="22" t="str">
+        <f>varsBy_room_cmp2!G7</f>
+        <v>2687</v>
+      </c>
+      <c r="J8" s="23" t="str">
+        <f>varsBy_room_cmp2!H7</f>
+        <v>(78.5%)</v>
+      </c>
+      <c r="K8" s="12" t="str">
+        <f>varsBy_room_cmp2!L7</f>
+        <v>&lt;0.0001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B9" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C9" s="7" t="str">
         <f>varsBy_room_cmp2!A10</f>
         <v>ims1</v>
       </c>
-      <c r="D8">
+      <c r="D9" s="7">
         <f>varsBy_room_cmp2!B10</f>
         <v>1</v>
       </c>
-      <c r="E8" s="14" t="str">
+      <c r="E9" s="9" t="str">
+        <f>varsBy_room_cmp2!C9</f>
+        <v>4.0</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f>varsBy_room_cmp2!D9</f>
+        <v>(2.0--9.0)</v>
+      </c>
+      <c r="G9" s="9" t="str">
+        <f>varsBy_room_cmp2!E9</f>
+        <v>2.0</v>
+      </c>
+      <c r="H9" s="20" t="str">
+        <f>varsBy_room_cmp2!F9</f>
+        <v>(1.0--7.0)</v>
+      </c>
+      <c r="I9" s="9" t="str">
+        <f>varsBy_room_cmp2!G9</f>
+        <v>2.0</v>
+      </c>
+      <c r="J9" s="20" t="str">
+        <f>varsBy_room_cmp2!H9</f>
+        <v>(1.0--5.0)</v>
+      </c>
+      <c r="K9" s="21" t="str">
+        <f>varsBy_room_cmp2!L9</f>
+        <v>&lt;0.0001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B10" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B11" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="10" t="str">
+        <f>varsBy_room_cmp2!A11</f>
+        <v>ims_delta</v>
+      </c>
+      <c r="D11" s="10">
+        <f>varsBy_room_cmp2!B11</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="22" t="str">
         <f>varsBy_room_cmp2!C10</f>
         <v>18.0</v>
       </c>
-      <c r="F8" t="str">
+      <c r="F11" s="23" t="str">
         <f>varsBy_room_cmp2!D10</f>
         <v>(12.0--23.0)</v>
       </c>
-      <c r="G8" s="15" t="str">
+      <c r="G11" s="22" t="str">
         <f>varsBy_room_cmp2!E10</f>
         <v>17.0</v>
       </c>
-      <c r="H8" t="str">
+      <c r="H11" s="23" t="str">
         <f>varsBy_room_cmp2!F10</f>
         <v>(12.0--22.0)</v>
       </c>
-      <c r="I8" s="15" t="str">
+      <c r="I11" s="22" t="str">
         <f>varsBy_room_cmp2!G10</f>
         <v>17.0</v>
       </c>
-      <c r="J8" t="str">
+      <c r="J11" s="23" t="str">
         <f>varsBy_room_cmp2!H10</f>
         <v>(12.0--23.0)</v>
       </c>
-      <c r="K8" s="15" t="str">
+      <c r="K11" s="12" t="str">
         <f>varsBy_room_cmp2!L10</f>
         <v>0.5996</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="13"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="C10" s="11" t="str">
-        <f>varsBy_room_cmp2!A11</f>
-        <v>ims_delta</v>
-      </c>
-      <c r="D10" s="11">
-        <f>varsBy_room_cmp2!B11</f>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B12" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="10" t="str">
+        <f>varsBy_room_cmp2!A12</f>
+        <v>alive7noICU</v>
+      </c>
+      <c r="D12" s="10">
+        <f>varsBy_room_cmp2!B12</f>
         <v>1</v>
       </c>
-      <c r="E10" s="12" t="str">
+      <c r="E12" s="22" t="str">
         <f>varsBy_room_cmp2!C11</f>
         <v>3.0</v>
       </c>
-      <c r="F10" s="11" t="str">
+      <c r="F12" s="23" t="str">
         <f>varsBy_room_cmp2!D11</f>
         <v>(-2.0--10.0)</v>
       </c>
-      <c r="G10" s="13" t="str">
+      <c r="G12" s="22" t="str">
         <f>varsBy_room_cmp2!E11</f>
         <v>3.0</v>
       </c>
-      <c r="H10" s="11" t="str">
+      <c r="H12" s="23" t="str">
         <f>varsBy_room_cmp2!F11</f>
         <v>(-3.0--9.0)</v>
       </c>
-      <c r="I10" s="13" t="str">
+      <c r="I12" s="22" t="str">
         <f>varsBy_room_cmp2!G11</f>
         <v>2.0</v>
       </c>
-      <c r="J10" s="11" t="str">
+      <c r="J12" s="23" t="str">
         <f>varsBy_room_cmp2!H11</f>
         <v>(-3.0--8.0)</v>
       </c>
-      <c r="K10" s="13" t="str">
+      <c r="K12" s="12" t="str">
         <f>varsBy_room_cmp2!L11</f>
         <v>0.0156</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="C11" s="11" t="str">
-        <f>varsBy_room_cmp2!A12</f>
-        <v>alive7noICU</v>
-      </c>
-      <c r="D11" s="11">
-        <f>varsBy_room_cmp2!B12</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="12" t="str">
-        <f>varsBy_room_cmp2!C12</f>
-        <v>143</v>
-      </c>
-      <c r="F11" s="11" t="str">
-        <f>varsBy_room_cmp2!D12</f>
-        <v>(38.0%)</v>
-      </c>
-      <c r="G11" s="13" t="str">
-        <f>varsBy_room_cmp2!E12</f>
-        <v>302</v>
-      </c>
-      <c r="H11" s="11" t="str">
-        <f>varsBy_room_cmp2!F12</f>
-        <v>(25.7%)</v>
-      </c>
-      <c r="I11" s="13" t="str">
-        <f>varsBy_room_cmp2!G12</f>
-        <v>618</v>
-      </c>
-      <c r="J11" s="11" t="str">
-        <f>varsBy_room_cmp2!H12</f>
-        <v>(18.1%)</v>
-      </c>
-      <c r="K11" s="13" t="str">
-        <f>varsBy_room_cmp2!L12</f>
-        <v>&lt;0.0001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>293</v>
-      </c>
-      <c r="E12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="K12" s="15"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
-        <v>294</v>
-      </c>
-      <c r="C13" t="str">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B13" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="K13" s="14"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B14" s="16" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="7" t="str">
         <f>varsBy_room_cmp2!A17</f>
         <v>dead7</v>
       </c>
-      <c r="D13">
+      <c r="D14" s="7">
         <f>varsBy_room_cmp2!B17</f>
         <v>0</v>
       </c>
-      <c r="E13" s="14" t="str">
-        <f>varsBy_room_cmp2!C17</f>
-        <v>303</v>
-      </c>
-      <c r="F13" t="str">
-        <f>varsBy_room_cmp2!D17</f>
-        <v>(80.6%)</v>
-      </c>
-      <c r="G13" s="15" t="str">
-        <f>varsBy_room_cmp2!E17</f>
-        <v>937</v>
-      </c>
-      <c r="H13" t="str">
-        <f>varsBy_room_cmp2!F17</f>
-        <v>(79.7%)</v>
-      </c>
-      <c r="I13" s="15" t="str">
-        <f>varsBy_room_cmp2!G17</f>
-        <v>2756</v>
-      </c>
-      <c r="J13" t="str">
-        <f>varsBy_room_cmp2!H17</f>
-        <v>(80.6%)</v>
-      </c>
-      <c r="K13" s="15">
-        <f>varsBy_room_cmp2!L17</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="C14" t="str">
+      <c r="E14" s="9" t="str">
+        <f>varsBy_room_cmp2!C16</f>
+        <v>73</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>varsBy_room_cmp2!D16</f>
+        <v>(19.4%)</v>
+      </c>
+      <c r="G14" s="9" t="str">
+        <f>varsBy_room_cmp2!E16</f>
+        <v>238</v>
+      </c>
+      <c r="H14" s="20" t="str">
+        <f>varsBy_room_cmp2!F16</f>
+        <v>(20.3%)</v>
+      </c>
+      <c r="I14" s="9" t="str">
+        <f>varsBy_room_cmp2!G16</f>
+        <v>665</v>
+      </c>
+      <c r="J14" s="20" t="str">
+        <f>varsBy_room_cmp2!H16</f>
+        <v>(19.4%)</v>
+      </c>
+      <c r="K14" s="21" t="str">
+        <f>varsBy_room_cmp2!L16</f>
+        <v>0.7427</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B15" s="16" t="s">
+        <v>292</v>
+      </c>
+      <c r="C15" s="7" t="str">
         <f>varsBy_room_cmp2!A15</f>
         <v>dead7noICU</v>
       </c>
-      <c r="D14">
+      <c r="D15" s="7">
         <f>varsBy_room_cmp2!B15</f>
         <v>0</v>
       </c>
-      <c r="E14" s="14" t="str">
-        <f>varsBy_room_cmp2!C15</f>
-        <v>344</v>
-      </c>
-      <c r="F14" t="str">
-        <f>varsBy_room_cmp2!D15</f>
-        <v>(91.5%)</v>
-      </c>
-      <c r="G14" s="15" t="str">
-        <f>varsBy_room_cmp2!E15</f>
-        <v>1105</v>
-      </c>
-      <c r="H14" t="str">
-        <f>varsBy_room_cmp2!F15</f>
-        <v>(94.0%)</v>
-      </c>
-      <c r="I14" s="15" t="str">
-        <f>varsBy_room_cmp2!G15</f>
-        <v>3305</v>
-      </c>
-      <c r="J14" t="str">
-        <f>varsBy_room_cmp2!H15</f>
-        <v>(96.6%)</v>
-      </c>
-      <c r="K14" s="15">
-        <f>varsBy_room_cmp2!L15</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C15" s="18" t="str">
+      <c r="E15" s="9" t="str">
+        <f>varsBy_room_cmp2!C14</f>
+        <v>32</v>
+      </c>
+      <c r="F15" s="20" t="str">
+        <f>varsBy_room_cmp2!D14</f>
+        <v>(8.5%)</v>
+      </c>
+      <c r="G15" s="9" t="str">
+        <f>varsBy_room_cmp2!E14</f>
+        <v>70</v>
+      </c>
+      <c r="H15" s="20" t="str">
+        <f>varsBy_room_cmp2!F14</f>
+        <v>(6.0%)</v>
+      </c>
+      <c r="I15" s="9" t="str">
+        <f>varsBy_room_cmp2!G14</f>
+        <v>116</v>
+      </c>
+      <c r="J15" s="20" t="str">
+        <f>varsBy_room_cmp2!H14</f>
+        <v>(3.4%)</v>
+      </c>
+      <c r="K15" s="21" t="str">
+        <f>varsBy_room_cmp2!L14</f>
+        <v>&lt;0.0001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B16" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="C16" s="17" t="str">
         <f>varsBy_room_cmp2!A19</f>
         <v>dead90</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D16" s="17">
         <f>varsBy_room_cmp2!B19</f>
         <v>0</v>
       </c>
-      <c r="E15" s="19" t="str">
-        <f>varsBy_room_cmp2!C19</f>
-        <v>243</v>
-      </c>
-      <c r="F15" s="18" t="str">
-        <f>varsBy_room_cmp2!D19</f>
-        <v>(64.6%)</v>
-      </c>
-      <c r="G15" s="20" t="str">
-        <f>varsBy_room_cmp2!E19</f>
-        <v>735</v>
-      </c>
-      <c r="H15" s="18" t="str">
-        <f>varsBy_room_cmp2!F19</f>
-        <v>(62.6%)</v>
-      </c>
-      <c r="I15" s="20" t="str">
-        <f>varsBy_room_cmp2!G19</f>
-        <v>2227</v>
-      </c>
-      <c r="J15" s="18" t="str">
-        <f>varsBy_room_cmp2!H19</f>
-        <v>(65.1%)</v>
-      </c>
-      <c r="K15" s="20">
-        <f>varsBy_room_cmp2!L19</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>298</v>
+      <c r="E16" s="18" t="str">
+        <f>varsBy_room_cmp2!C18</f>
+        <v>133</v>
+      </c>
+      <c r="F16" s="24" t="str">
+        <f>varsBy_room_cmp2!D18</f>
+        <v>(35.4%)</v>
+      </c>
+      <c r="G16" s="18" t="str">
+        <f>varsBy_room_cmp2!E18</f>
+        <v>440</v>
+      </c>
+      <c r="H16" s="24" t="str">
+        <f>varsBy_room_cmp2!F18</f>
+        <v>(37.4%)</v>
+      </c>
+      <c r="I16" s="18" t="str">
+        <f>varsBy_room_cmp2!G18</f>
+        <v>1194</v>
+      </c>
+      <c r="J16" s="24" t="str">
+        <f>varsBy_room_cmp2!H18</f>
+        <v>(34.9%)</v>
+      </c>
+      <c r="K16" s="18" t="str">
+        <f>varsBy_room_cmp2!L18</f>
+        <v>0.3145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="7" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="7" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>